<commit_message>
ERC and DRC passed. BOM not quite done
</commit_message>
<xml_diff>
--- a/FLCOS Projector BOM 5-10-22.xlsx
+++ b/FLCOS Projector BOM 5-10-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EAGLE 9.0.1\projects\examples\FLCOS Projector Driver - Common-Anode, ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8EE8B7-6927-452E-BF6B-E12A77AD74CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06831E1-1A5C-4FA3-8ABE-C1E2F9B8B8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7665" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,10 +19,18 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'FLCOS Projector Driver BOM'!$A$1:$K$32</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="169">
   <si>
     <t>Column1</t>
   </si>
@@ -126,9 +134,6 @@
     <t>C-EUC0603</t>
   </si>
   <si>
-    <t>10pF</t>
-  </si>
-  <si>
     <t>C49</t>
   </si>
   <si>
@@ -189,9 +194,6 @@
     <t>SO08-PAD</t>
   </si>
   <si>
-    <t>MIC5219BM5</t>
-  </si>
-  <si>
     <t>SOT23-5</t>
   </si>
   <si>
@@ -259,12 +261,6 @@
   </si>
   <si>
     <t>37R5</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>0R</t>
   </si>
   <si>
     <t>470R</t>
@@ -422,9 +418,6 @@
     <t>ECS</t>
   </si>
   <si>
-    <t>L1, L2, L5</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Laird-Performance-Materials/TYS6028150M-10?qs=cCJXSq33DMHy4lem%252B%252BTS7Q%3D%3D</t>
   </si>
   <si>
@@ -474,16 +467,7 @@
     <t>https://www.mouser.com/ProductDetail/Micro-Commercial-Components-MCC/MMSS8050-H-TP?qs=FaVZESsvgndwiDXxXq5g0g%3D%3D</t>
   </si>
   <si>
-    <t>C13, C18, C20, C21, C22, C23, C47, C50, C55, C56</t>
-  </si>
-  <si>
-    <t>C14, C15</t>
-  </si>
-  <si>
     <t>C1, C2, C16, C17, C19, C27</t>
-  </si>
-  <si>
-    <t>C52, C53</t>
   </si>
   <si>
     <t>D1, D2, D3</t>
@@ -499,9 +483,6 @@
 SB34AFC-AU_R1_000A1</t>
   </si>
   <si>
-    <t>IC2, IC3</t>
-  </si>
-  <si>
     <t>IC7, IC8, IC9</t>
   </si>
   <si>
@@ -511,9 +492,6 @@
     <t>R2, R4, R16</t>
   </si>
   <si>
-    <t>R7, R8, R9, R10</t>
-  </si>
-  <si>
     <t>R62, R63</t>
   </si>
   <si>
@@ -536,6 +514,48 @@
   </si>
   <si>
     <t>X2</t>
+  </si>
+  <si>
+    <t>L1, L2, L3</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>R7, R8, R9, R10, R11</t>
+  </si>
+  <si>
+    <t>C14, C15, C52, C53</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>MIC5323-1.8YD5-TR</t>
+  </si>
+  <si>
+    <t>MIC5504-2.5YM5-TR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Microchip-Technology-Atmel/MIC5323-1.8YD5-TR?qs=U6T8BxXiZAV5mWt%252BoHf49w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Microchip-Technology-Atmel/MIC5504-2.5YM5-TR?qs=U6T8BxXiZAXfKTfMymzCuw%3D%3D</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>998-MIC5504-2.5YM5TR</t>
+  </si>
+  <si>
+    <t>998-MIC5323-1.8YD5TR</t>
+  </si>
+  <si>
+    <t>C3, C13, C18, C20, C21, C22, C23, C47, C50, C55, C56</t>
   </si>
 </sst>
 </file>
@@ -543,7 +563,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -574,52 +594,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-409]#,##0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -630,55 +619,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{E109AA8F-2CDC-40FC-B6B4-8AC572338037}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="19">
-    <queryTableFields count="11">
-      <queryTableField id="1" name="Column1" tableColumnId="1"/>
-      <queryTableField id="2" name="Column2" tableColumnId="2"/>
-      <queryTableField id="3" name="Column3" tableColumnId="3"/>
-      <queryTableField id="4" name="Column4" tableColumnId="4"/>
-      <queryTableField id="5" name="Column5" tableColumnId="5"/>
-      <queryTableField id="6" name="Column6" tableColumnId="6"/>
-      <queryTableField id="7" name="Column7" tableColumnId="7"/>
-      <queryTableField id="8" name="Column8" tableColumnId="8"/>
-      <queryTableField id="9" name="Column9" tableColumnId="9"/>
-      <queryTableField id="11" name="Column11" tableColumnId="11"/>
-      <queryTableField id="12" name="Column12" tableColumnId="12"/>
-    </queryTableFields>
-    <queryTableDeletedFields count="7">
-      <deletedField name="Column10"/>
-      <deletedField name="Column13"/>
-      <deletedField name="Column14"/>
-      <deletedField name="Column15"/>
-      <deletedField name="Column16"/>
-      <deletedField name="Column17"/>
-      <deletedField name="Column18"/>
-    </queryTableDeletedFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EC0F30C-DCE0-4E7D-9569-5E6F235D0228}" name="FLCOS_Projector_Driver_BOM" displayName="FLCOS_Projector_Driver_BOM" ref="A1:K33" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:K33" xr:uid="{4EC0F30C-DCE0-4E7D-9569-5E6F235D0228}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{6FD76936-DB64-417E-83AC-AC1CD46B5279}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{622E6FDD-EF89-4AE9-B6D8-20AC9A80C5A1}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{376690AA-7EA8-4DFB-872A-E67D530B0F7E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{41FFA62C-14A0-4310-97DB-391A6E8324A4}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{6B705877-E486-41D4-8784-CD4CB17DEFBF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{7C62B2A2-16F6-430D-8DEA-25B971379DC2}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{782683D7-1311-4E6E-8240-F48B3C41B737}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{339BC429-9146-4001-A966-A18B48469FA7}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{612B790E-BA5F-45F0-853E-737B79777F2E}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{DDC414FB-0234-4F92-A369-C7D1DD546876}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{73D12149-25DD-486F-933D-02251F121B1C}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -944,15 +884,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990DCC5F-A888-4D41-9D9F-7B39C31D0DA6}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="42.921875" customWidth="1"/>
+    <col min="1" max="1" width="45.69140625" customWidth="1"/>
     <col min="2" max="2" width="22.07421875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.3046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.15234375" bestFit="1" customWidth="1"/>
@@ -1037,21 +977,6 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1073,13 +998,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>25</v>
@@ -1108,10 +1033,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>28</v>
@@ -1143,10 +1068,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -1178,54 +1103,36 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1236,36 +1143,36 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1276,19 +1183,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1299,19 +1206,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1322,357 +1229,411 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K16" s="3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K18" s="3">
-        <v>5.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0.45</v>
+      <c r="D19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.21</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="K21" s="3">
-        <v>0.21</v>
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>163</v>
+      </c>
+      <c r="H22" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.68</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>162</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>122</v>
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>164</v>
+      </c>
+      <c r="H23" t="s">
+        <v>165</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="K23" s="3">
-        <v>1.77</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A25" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K25" s="3">
-        <v>2.48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" s="3">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="3">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K27" s="3">
-        <v>6.56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K28" s="3">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="G30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>136</v>
+        <v>109</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="K30" s="3">
-        <v>1.96</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>99</v>
@@ -1681,150 +1642,150 @@
         <v>99</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>22</v>
+        <v>108</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K31" s="3">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A32" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="1" t="s">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K32" s="3">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K33" s="3">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="K34" s="3">
-        <v>1.1299999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K35" s="3">
         <v>0.37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>22</v>
@@ -1847,19 +1808,19 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>22</v>
@@ -1880,47 +1841,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>22</v>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J44" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K44" s="3">
+        <f>SUM(K3:K41)</f>
+        <v>20.602999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed to USB-C. BOM passives not done yet
</commit_message>
<xml_diff>
--- a/FLCOS Projector BOM 5-10-22.xlsx
+++ b/FLCOS Projector BOM 5-10-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EAGLE 9.0.1\projects\examples\FLCOS Projector Driver - Common-Anode, ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06831E1-1A5C-4FA3-8ABE-C1E2F9B8B8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC300195-6E00-45A8-AFF6-B4628C367DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7665" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -248,9 +248,6 @@
     <t>RESISTOR, American symbol</t>
   </si>
   <si>
-    <t>20K</t>
-  </si>
-  <si>
     <t>2K2</t>
   </si>
   <si>
@@ -329,18 +326,6 @@
     <t>SOIC16</t>
   </si>
   <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>MINI-USB-32005-301</t>
-  </si>
-  <si>
-    <t>32005-301</t>
-  </si>
-  <si>
-    <t>MINI USB-B Conector</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -365,19 +350,10 @@
     <t>https://www.mouser.com/ProductDetail/ECS/ECS-120-12-36-AGN-TR3?qs=sGAEpiMZZMsBj6bBr9Q9aVdL36W7rCWD8CqL8fyXs5WE4m0aT%2FQX9w%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/CUI-Devices/UJ2-MBH-1-SMT-TR?qs=5mqXD9RfOg2uumvPfpWvPw%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Amphenol-FCI/SFV25R-2STE1HLF?qs=SqJKR5MmrydEjQnFJmTcbQ%3D%3D</t>
   </si>
   <si>
     <t>Top Contact!</t>
-  </si>
-  <si>
-    <t>CUI</t>
-  </si>
-  <si>
-    <t>490-UJ2-MBH-1-SMT</t>
   </si>
   <si>
     <t>520-ECS143-20-23A-EN</t>
@@ -387,9 +363,6 @@
 ESP32-WROOM-32UE-N16</t>
   </si>
   <si>
-    <t>UJ2-MBH-1-SMT-TR</t>
-  </si>
-  <si>
     <t>649-SFV25R-2STE1HLF</t>
   </si>
   <si>
@@ -442,10 +415,6 @@
     <t>GCT</t>
   </si>
   <si>
-    <t xml:space="preserve">
-MEM2075-00-140-01-A</t>
-  </si>
-  <si>
     <t>640-MEM20750014001A</t>
   </si>
   <si>
@@ -489,9 +458,6 @@
     <t>R1, R3, R15</t>
   </si>
   <si>
-    <t>R2, R4, R16</t>
-  </si>
-  <si>
     <t>R62, R63</t>
   </si>
   <si>
@@ -556,6 +522,40 @@
   </si>
   <si>
     <t>C3, C13, C18, C20, C21, C22, C23, C47, C50, C55, C56</t>
+  </si>
+  <si>
+    <t>Panjit</t>
+  </si>
+  <si>
+    <t>USB-C</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/GCT/USB4105-GF-A?qs=KUoIvG%2F9IlY%2FMLlBMpStpA%3D%3D</t>
+  </si>
+  <si>
+    <t>USB-C connector</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>GCT_USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>USB Type C,2.0</t>
+  </si>
+  <si>
+    <t>640-USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>MEM2075-00-140-01-A
+MEM2075-00-140-01-A</t>
+  </si>
+  <si>
+    <t>22K</t>
+  </si>
+  <si>
+    <t>R2, R4, R13, R14, R16</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -998,7 +998,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>27</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>63</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>167</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>64</v>
@@ -1160,19 +1160,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1183,19 +1183,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1206,19 +1206,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1229,19 +1229,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -1254,7 +1254,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>54</v>
@@ -1269,19 +1269,19 @@
         <v>57</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="K16" s="3">
         <v>5.2999999999999999E-2</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="18" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -1304,19 +1304,19 @@
         <v>41</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="K18" s="3">
         <v>0.45</v>
@@ -1324,34 +1324,34 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="K19" s="3">
         <v>0.21</v>
@@ -1362,7 +1362,7 @@
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>43</v>
@@ -1374,19 +1374,19 @@
         <v>45</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="K21" s="3">
         <v>1.77</v>
@@ -1394,13 +1394,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>49</v>
@@ -1409,16 +1409,16 @@
         <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="H22" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="K22" s="3">
         <v>0.68</v>
@@ -1426,13 +1426,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>49</v>
@@ -1441,16 +1441,16 @@
         <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="H23" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="K23" s="3">
         <v>0.16</v>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>46</v>
@@ -1473,19 +1473,19 @@
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="J24" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="K24" s="3">
         <v>2.48</v>
@@ -1496,19 +1496,19 @@
         <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>22</v>
@@ -1517,10 +1517,10 @@
         <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K26" s="3">
         <v>6.56</v>
@@ -1531,31 +1531,31 @@
         <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="K27" s="3">
         <v>3.6</v>
@@ -1563,34 +1563,34 @@
     </row>
     <row r="29" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="K29" s="3">
         <v>1.96</v>
@@ -1598,34 +1598,34 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="K30" s="3">
         <v>0.56000000000000005</v>
@@ -1633,42 +1633,42 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="K31" s="3">
-        <v>0.62</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>58</v>
@@ -1683,19 +1683,19 @@
         <v>61</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K33" s="3">
         <v>1.1299999999999999</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="34" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>62</v>
@@ -1718,19 +1718,19 @@
         <v>61</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="K34" s="3">
         <v>0.37</v>
@@ -1741,13 +1741,13 @@
         <v>52</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>22</v>
@@ -1773,16 +1773,16 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>22</v>
@@ -1843,11 +1843,11 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J44" s="4" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="K44" s="3">
         <f>SUM(K3:K41)</f>
-        <v>20.602999999999998</v>
+        <v>20.792999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Composite pin header for TRRS socket
</commit_message>
<xml_diff>
--- a/FLCOS Projector BOM 5-10-22.xlsx
+++ b/FLCOS Projector BOM 5-10-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EAGLE 9.0.1\projects\examples\FLCOS Projector Driver - Common-Anode, ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC300195-6E00-45A8-AFF6-B4628C367DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF8906B-83C9-4840-BA4C-CF56966EE71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7665" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="173">
   <si>
     <t>Column1</t>
   </si>
@@ -155,13 +155,7 @@
     <t>CVBS</t>
   </si>
   <si>
-    <t>PINHD-1X3</t>
-  </si>
-  <si>
     <t>1X03</t>
-  </si>
-  <si>
-    <t>PIN HEADER</t>
   </si>
   <si>
     <t>DIODE-SCHOTTKYSMA</t>
@@ -556,6 +550,24 @@
   </si>
   <si>
     <t>R2, R4, R13, R14, R16</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SparkFun/PRT-12639?qs=WyAARYrbSnautCwYhJcFjA%3D%3D</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>PRT-12639</t>
+  </si>
+  <si>
+    <t>474-PRT-12639</t>
+  </si>
+  <si>
+    <t>AUDIO_JACK_TRRSSMD_RA</t>
+  </si>
+  <si>
+    <t>Audio Jack 3.5mm TRRS</t>
   </si>
 </sst>
 </file>
@@ -887,13 +899,13 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="45.69140625" customWidth="1"/>
-    <col min="2" max="2" width="22.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.15234375" customWidth="1"/>
     <col min="3" max="3" width="27.3046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.15234375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
@@ -998,7 +1010,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
@@ -1033,7 +1045,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>27</v>
@@ -1068,7 +1080,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
@@ -1120,19 +1132,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1143,36 +1155,36 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1183,19 +1195,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1206,19 +1218,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1229,19 +1241,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -1254,34 +1266,34 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="I16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="K16" s="3">
         <v>5.2999999999999999E-2</v>
@@ -1289,34 +1301,34 @@
     </row>
     <row r="18" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="K18" s="3">
         <v>0.45</v>
@@ -1324,34 +1336,34 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="J19" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K19" s="3">
         <v>0.21</v>
@@ -1359,34 +1371,34 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="F21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="K21" s="3">
         <v>1.77</v>
@@ -1394,31 +1406,31 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>152</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="K22" s="3">
         <v>0.68</v>
@@ -1426,31 +1438,31 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="H23" t="s">
-        <v>154</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="K23" s="3">
         <v>0.16</v>
@@ -1458,34 +1470,34 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K24" s="3">
         <v>2.48</v>
@@ -1493,22 +1505,22 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>22</v>
@@ -1517,10 +1529,10 @@
         <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K26" s="3">
         <v>6.56</v>
@@ -1528,34 +1540,34 @@
     </row>
     <row r="27" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="I27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="K27" s="3">
         <v>3.6</v>
@@ -1563,34 +1575,34 @@
     </row>
     <row r="29" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="F29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="K29" s="3">
         <v>1.96</v>
@@ -1598,34 +1610,34 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="K30" s="3">
         <v>0.56000000000000005</v>
@@ -1633,34 +1645,34 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K31" s="3">
         <v>0.81</v>
@@ -1668,34 +1680,34 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K33" s="3">
         <v>1.1299999999999999</v>
@@ -1703,151 +1715,151 @@
     </row>
     <row r="34" spans="1:11" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K34" s="3">
         <v>0.37</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>22</v>
+        <v>172</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>22</v>
+        <v>168</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K38" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J44" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K44" s="3">
         <f>SUM(K3:K41)</f>
-        <v>20.792999999999996</v>
+        <v>21.742999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Mouser cart XLS. BOM tweaks due to low stocks
</commit_message>
<xml_diff>
--- a/FLCOS Projector BOM 5-10-22.xlsx
+++ b/FLCOS Projector BOM 5-10-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EAGLE 9.0.1\projects\examples\FLCOS Projector Driver - Common-Anode, ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99739A7B-A3D8-4EB5-AED2-7EFEAFBF7552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75C82C4-5649-479D-B435-72A248F26CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7665" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="215">
   <si>
     <t>Part</t>
   </si>
@@ -134,9 +134,6 @@
     <t>SOT223</t>
   </si>
   <si>
-    <t>Voltage Regulator LM1117</t>
-  </si>
-  <si>
     <t>LM3414</t>
   </si>
   <si>
@@ -245,16 +242,10 @@
     <t>TQFP32-5MM</t>
   </si>
   <si>
-    <t>ESP32-WROOM-32U</t>
-  </si>
-  <si>
     <t>ESP32WROOM32D</t>
   </si>
   <si>
     <t>Espressif</t>
-  </si>
-  <si>
-    <t>356-ESP32-WROOM-32U</t>
   </si>
   <si>
     <t>CH340G</t>
@@ -395,15 +386,6 @@
   </si>
   <si>
     <t>R5, R6, R12, R67</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/LM1117MPX-3.3?qs=X1J7HmVL2ZF%2FbtmfJGRL0w%3D%3D</t>
-  </si>
-  <si>
-    <t>LM1117MPX-3.3</t>
-  </si>
-  <si>
-    <t>926-LM1117MPX-33</t>
   </si>
   <si>
     <t>FPC</t>
@@ -547,9 +529,6 @@
     <t>187-CL10C220JB8NNWC</t>
   </si>
   <si>
-    <t>ESP32-D0WD, 32Mbits SPI flash, U.FL antenna</t>
-  </si>
-  <si>
     <t>C3, C13, C18, C20, C21, C22, C23, C47, C50, C56</t>
   </si>
   <si>
@@ -689,6 +668,33 @@
   </si>
   <si>
     <t>USB UART IC. SOIC16 package.</t>
+  </si>
+  <si>
+    <t>SCHOTTKY</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TLV1117LV33DCYT?qs=tEz3BkPb1ry8fvdWR4Nyog%3D%3D</t>
+  </si>
+  <si>
+    <t>TLV1117LV33DCYT</t>
+  </si>
+  <si>
+    <t>595-TLV1117LV33DCYT</t>
+  </si>
+  <si>
+    <t>Voltage Regulator TLV1117. 1 Amp. Pos.</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32UE-N4</t>
+  </si>
+  <si>
+    <t>356-ESP32WRM32UE32UH</t>
+  </si>
+  <si>
+    <t>ESP32-D0WD, 4Mbits SPI flash, U.FL antenna</t>
+  </si>
+  <si>
+    <t>Not commonly available from western distributors. May need to buy on eBay, Amazon, AliExpress. Sparkfun sell the CH340E (different package), but only in quantity 10.</t>
   </si>
 </sst>
 </file>
@@ -1027,18 +1033,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990DCC5F-A888-4D41-9D9F-7B39C31D0DA6}">
   <dimension ref="A2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="40.3046875" customWidth="1"/>
-    <col min="2" max="2" width="23.69140625" customWidth="1"/>
-    <col min="3" max="3" width="27.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.15234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.15234375" customWidth="1"/>
-    <col min="6" max="6" width="10.23046875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="38.69140625" customWidth="1"/>
+    <col min="2" max="2" width="10.07421875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.69140625" customWidth="1"/>
+    <col min="4" max="4" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.15234375" customWidth="1"/>
     <col min="7" max="8" width="15.69140625" style="4" customWidth="1"/>
     <col min="9" max="9" width="22.53515625" customWidth="1"/>
     <col min="10" max="10" width="28.4609375" customWidth="1"/>
@@ -1054,26 +1060,26 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
@@ -1085,7 +1091,7 @@
         <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
@@ -1108,444 +1114,444 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="4">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" s="4">
-        <v>6</v>
       </c>
       <c r="G4" s="5">
         <v>0.1</v>
       </c>
       <c r="H4" s="5">
-        <f>F4*G4</f>
+        <f>B4*G4</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="4">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F5" s="4">
-        <v>11</v>
       </c>
       <c r="G5" s="5">
         <v>0.1</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" ref="H5:H44" si="0">F5*G5</f>
-        <v>1.1000000000000001</v>
+        <f>B5*G5</f>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4</v>
       </c>
       <c r="G6" s="5">
         <v>0.1</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" si="0"/>
+        <f>B6*G6</f>
         <v>0.4</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
       </c>
       <c r="G7" s="5">
         <v>0.37</v>
       </c>
       <c r="H7" s="5">
-        <f>F7*G7</f>
+        <f>B7*G7</f>
         <v>0.37</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="L7" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
       </c>
       <c r="G8" s="5">
         <v>0.67</v>
       </c>
       <c r="H8" s="5">
-        <f>F8*G8</f>
+        <f>B8*G8</f>
         <v>0.67</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="L8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G9" s="5"/>
       <c r="H9" s="5">
-        <f t="shared" si="0"/>
+        <f>B9*G9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>178</v>
+        <v>109</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="4">
-        <v>3</v>
       </c>
       <c r="G10" s="5">
         <v>0.1</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="0"/>
+        <f>B10*G10</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
+      </c>
+      <c r="B11" s="4">
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="4">
-        <v>5</v>
       </c>
       <c r="G11" s="5">
         <v>0.12</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="0"/>
+        <f>B11*G11</f>
         <v>0.6</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="L11" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="4">
-        <v>4</v>
       </c>
       <c r="G12" s="5">
         <v>0.11</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="0"/>
+        <f>B12*G12</f>
         <v>0.44</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>189</v>
+        <v>117</v>
+      </c>
+      <c r="B13" s="4">
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="4">
-        <v>5</v>
       </c>
       <c r="G13" s="5">
         <v>0.1</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="0"/>
+        <f>B13*G13</f>
         <v>0.5</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>110</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="4">
-        <v>2</v>
       </c>
       <c r="G14" s="5">
         <v>0.1</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="0"/>
+        <f>B14*G14</f>
         <v>0.2</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>111</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2</v>
       </c>
       <c r="G15" s="5">
         <v>0.1</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="0"/>
+        <f>B15*G15</f>
         <v>0.2</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="L15" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G16" s="5"/>
       <c r="H16" s="5">
-        <f t="shared" si="0"/>
+        <f>B16*G16</f>
         <v>0</v>
       </c>
       <c r="I16" s="1"/>
@@ -1555,132 +1561,132 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="4">
-        <v>3</v>
       </c>
       <c r="G17" s="5">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="0"/>
+        <f>B17*G17</f>
         <v>0.159</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G18" s="5"/>
       <c r="H18" s="5">
-        <f t="shared" si="0"/>
+        <f>B18*G18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>104</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F19" s="4">
-        <v>3</v>
       </c>
       <c r="G19" s="5">
         <v>0.45</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="0"/>
+        <f>B19*G19</f>
         <v>1.35</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="4">
-        <v>2</v>
       </c>
       <c r="G20" s="5">
         <v>0.21</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="0"/>
+        <f>B20*G20</f>
         <v>0.42</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G21" s="5"/>
       <c r="H21" s="5">
-        <f t="shared" si="0"/>
+        <f>B21*G21</f>
         <v>0</v>
       </c>
     </row>
@@ -1688,456 +1694,456 @@
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>117</v>
+      <c r="B22" s="4">
+        <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="4">
-        <v>1</v>
+      <c r="F22" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="G22" s="5">
-        <v>1.77</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="0"/>
-        <v>1.77</v>
+        <f>B22*G22</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>117</v>
+        <v>208</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>118</v>
+        <v>209</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="4">
-        <v>1</v>
       </c>
       <c r="G23" s="5">
         <v>0.68</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="0"/>
+        <f>B23*G23</f>
         <v>0.68</v>
       </c>
       <c r="I23" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="L23" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1</v>
       </c>
       <c r="G24" s="5">
         <v>0.16</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="0"/>
+        <f>B24*G24</f>
         <v>0.16</v>
       </c>
       <c r="I24" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L24" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="4">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F25" s="4">
-        <v>3</v>
       </c>
       <c r="G25" s="5">
         <v>2.48</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="0"/>
+        <f>B25*G25</f>
         <v>7.4399999999999995</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G26" s="5"/>
       <c r="H26" s="5">
-        <f t="shared" si="0"/>
+        <f>B26*G26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
+      <c r="F27" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="G27" s="5">
         <v>6.56</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="0"/>
+        <f>B27*G27</f>
         <v>6.56</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G28" s="5">
+        <v>3</v>
+      </c>
+      <c r="H28" s="5">
+        <f>B28*G28</f>
+        <v>3</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="5">
-        <v>3.6</v>
-      </c>
-      <c r="H28" s="5">
-        <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>66</v>
+        <v>211</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>69</v>
+        <v>212</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G29" s="5"/>
       <c r="H29" s="5">
-        <f t="shared" si="0"/>
+        <f>B29*G29</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="4">
-        <v>1</v>
       </c>
       <c r="G30" s="5">
         <v>1.96</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="0"/>
+        <f>B30*G30</f>
         <v>1.96</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F31" s="4">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="G31" s="5">
         <v>0.56000000000000005</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" si="0"/>
+        <f>B31*G31</f>
         <v>0.56000000000000005</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>113</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="4">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="G32" s="5">
         <v>0.81</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" si="0"/>
+        <f>B32*G32</f>
         <v>0.81</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G33" s="5"/>
       <c r="H33" s="5">
-        <f t="shared" si="0"/>
+        <f>B33*G33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1</v>
       </c>
       <c r="G34" s="5">
         <v>1.1299999999999999</v>
       </c>
       <c r="H34" s="5">
-        <f t="shared" si="0"/>
+        <f>B34*G34</f>
         <v>1.1299999999999999</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>46</v>
+        <v>114</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="4">
-        <v>1</v>
       </c>
       <c r="G35" s="5">
         <v>0.37</v>
       </c>
       <c r="H35" s="5">
-        <f t="shared" si="0"/>
+        <f>B35*G35</f>
         <v>0.37</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G36" s="5"/>
       <c r="H36" s="5">
-        <f t="shared" si="0"/>
+        <f>B36*G36</f>
         <v>0</v>
       </c>
     </row>
@@ -2145,213 +2151,213 @@
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>149</v>
+      <c r="B37" s="4">
+        <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F37" s="4">
-        <v>1</v>
+      <c r="F37" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="G37" s="5">
         <v>0.95</v>
       </c>
       <c r="H37" s="5">
-        <f t="shared" si="0"/>
+        <f>B37*G37</f>
         <v>0.95</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G38" s="5"/>
       <c r="H38" s="5">
-        <f t="shared" si="0"/>
+        <f>B38*G38</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G39" s="5"/>
       <c r="H39" s="5">
-        <f t="shared" si="0"/>
+        <f>B39*G39</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>35</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F40" s="4">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="G40" s="5">
         <v>0</v>
       </c>
       <c r="H40" s="5">
-        <f t="shared" si="0"/>
+        <f>B40*G40</f>
         <v>0</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F41" s="4">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="G41" s="5">
         <v>0</v>
       </c>
       <c r="H41" s="5">
-        <f t="shared" si="0"/>
+        <f>B41*G41</f>
         <v>0</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G42" s="5"/>
       <c r="H42" s="5">
-        <f t="shared" si="0"/>
+        <f>B42*G42</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>202</v>
-      </c>
-      <c r="B43" t="s">
-        <v>202</v>
+        <v>195</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D43" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E43" t="s">
-        <v>203</v>
-      </c>
-      <c r="F43" s="4">
-        <v>1</v>
+        <v>195</v>
+      </c>
+      <c r="F43" t="s">
+        <v>196</v>
       </c>
       <c r="G43" s="5">
         <v>0.497</v>
       </c>
       <c r="H43" s="5">
-        <f t="shared" si="0"/>
+        <f>B43*G43</f>
         <v>0.497</v>
       </c>
       <c r="I43" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="L43" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>204</v>
-      </c>
-      <c r="B44" t="s">
-        <v>206</v>
+        <v>197</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D44" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E44" t="s">
-        <v>205</v>
-      </c>
-      <c r="F44" s="4">
-        <v>1</v>
+        <v>199</v>
+      </c>
+      <c r="F44" t="s">
+        <v>198</v>
       </c>
       <c r="G44" s="5">
         <v>6.95</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" si="0"/>
+        <f>B44*G44</f>
         <v>6.95</v>
       </c>
       <c r="I44" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="L44" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G46" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H46" s="5">
         <f>SUM(H4:H44)</f>
-        <v>40.746000000000002</v>
+        <v>39.415999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>